<commit_message>
[BAF510] : 채권 hw2 par yield & zero 엑셀 풀이 중
</commit_message>
<xml_diff>
--- a/BAF510채권/T2.xlsx
+++ b/BAF510채권/T2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\KAIST_MFE\sem1.1\BAF510채권분석\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chlje\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A25E8A-A2EE-45AE-B10F-A5A5B3DC19DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C62B48-6593-45EF-8951-A9D59C5EDDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price" sheetId="1" r:id="rId1"/>
@@ -36402,14 +36402,14 @@
         <v>20</v>
       </c>
       <c r="L30" s="1">
-        <f t="dataTable" ref="L30:L70" dt2D="0" dtr="0" r1="I27"/>
+        <f t="dataTable" ref="L30:L70" dt2D="0" dtr="0" r1="I27" ca="1"/>
         <v>1220.9983991771542</v>
       </c>
       <c r="O30">
         <v>0.01</v>
       </c>
       <c r="P30">
-        <f t="dataTable" ref="P30:P52" dt2D="0" dtr="0" r1="I30" ca="1"/>
+        <f t="dataTable" ref="P30:P52" dt2D="0" dtr="0" r1="I30"/>
         <v>1854.4338616001187</v>
       </c>
     </row>
@@ -50801,14 +50801,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="C246">
-        <f t="dataTable" ref="C246:C258" dt2D="0" dtr="0" r1="C237"/>
+        <f t="dataTable" ref="C246:C258" dt2D="0" dtr="0" r1="C237" ca="1"/>
         <v>1631.5889067095873</v>
       </c>
       <c r="E246">
         <v>0</v>
       </c>
       <c r="F246">
-        <f t="dataTable" ref="F246:F258" dt2D="0" dtr="0" r1="C235" ca="1"/>
+        <f t="dataTable" ref="F246:F258" dt2D="0" dtr="0" r1="C235"/>
         <v>3351.5716215288121</v>
       </c>
     </row>
@@ -51983,8 +51983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:Q139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H143" sqref="H143"/>
+    <sheetView tabSelected="1" topLeftCell="C99" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108:I124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
[BAF510] : 채권 hw2 Notability 손글씨 포함 최종본 완성
</commit_message>
<xml_diff>
--- a/BAF510채권/T2.xlsx
+++ b/BAF510채권/T2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chlje\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C62B48-6593-45EF-8951-A9D59C5EDDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6A6A90-90BB-4E9D-AB7D-79C789D13B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price" sheetId="1" r:id="rId1"/>
@@ -115,8 +115,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -124,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="298">
   <si>
     <t xml:space="preserve">frequency </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1287,6 +1285,9 @@
   <si>
     <t>pv</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product2</t>
   </si>
 </sst>
 </file>
@@ -35824,16 +35825,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>52916</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>62439</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>444499</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>178855</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>243416</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>116416</xdr:colOff>
       <xdr:row>123</xdr:row>
-      <xdr:rowOff>158748</xdr:rowOff>
+      <xdr:rowOff>84664</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -36200,14 +36201,14 @@
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="33.6">
+    <row r="2" spans="2:4" ht="33.75">
       <c r="B2" s="15" t="s">
         <v>292</v>
       </c>
@@ -36300,7 +36301,7 @@
         <v>1156.8950957737293</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="15" thickBot="1"/>
+    <row r="25" spans="2:16" ht="15.75" thickBot="1"/>
     <row r="26" spans="2:16">
       <c r="B26" s="2" t="s">
         <v>3</v>
@@ -36378,7 +36379,7 @@
         <v>1150.8261172101793</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="15" thickBot="1">
+    <row r="30" spans="2:16" ht="15.75" thickBot="1">
       <c r="B30" s="6" t="s">
         <v>7</v>
       </c>
@@ -36413,7 +36414,7 @@
         <v>1854.4338616001187</v>
       </c>
     </row>
-    <row r="31" spans="2:16" ht="15" thickBot="1">
+    <row r="31" spans="2:16" ht="15.75" thickBot="1">
       <c r="E31">
         <v>19.5</v>
       </c>
@@ -36603,7 +36604,7 @@
         <v>1490.5430003379133</v>
       </c>
     </row>
-    <row r="37" spans="2:16" ht="15" thickBot="1">
+    <row r="37" spans="2:16" ht="15.75" thickBot="1">
       <c r="B37" s="6" t="s">
         <v>10</v>
       </c>
@@ -37205,17 +37206,17 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1"/>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:12">
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -37249,7 +37250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="43.2">
+    <row r="5" spans="2:12" ht="45">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -37281,7 +37282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="15" thickBot="1">
+    <row r="6" spans="2:12" ht="15.75" thickBot="1">
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
@@ -37320,7 +37321,7 @@
         <v>940.37050780850541</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15" thickBot="1">
+    <row r="7" spans="2:12" ht="15.75" thickBot="1">
       <c r="E7">
         <f>E6-0.1</f>
         <v>9.8000000000000007</v>
@@ -37559,7 +37560,7 @@
         <v>942.3526434574311</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="15" thickBot="1">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1">
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
@@ -40709,21 +40710,21 @@
       <selection activeCell="G267" sqref="G267"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="33.6">
+    <row r="2" spans="2:10" ht="33.75">
       <c r="B2" s="15" t="s">
         <v>29</v>
       </c>
@@ -40973,12 +40974,12 @@
         <v>-210.19876543209875</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="33.6">
+    <row r="30" spans="2:10" ht="33.75">
       <c r="B30" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="43.2">
+    <row r="33" spans="2:8" ht="45">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -41197,7 +41198,7 @@
         <v>6492830.2486569844</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="33.6">
+    <row r="51" spans="2:12" ht="33.75">
       <c r="B51" s="15" t="s">
         <v>40</v>
       </c>
@@ -42066,7 +42067,7 @@
     <row r="86" spans="2:12">
       <c r="D86" s="19"/>
     </row>
-    <row r="89" spans="2:12" ht="33.6">
+    <row r="89" spans="2:12" ht="33.75">
       <c r="B89" s="15" t="s">
         <v>50</v>
       </c>
@@ -42350,7 +42351,7 @@
         <v>-5.8692194215836935E-7</v>
       </c>
     </row>
-    <row r="113" spans="2:11" ht="33.6">
+    <row r="113" spans="2:11" ht="33.75">
       <c r="B113" s="15" t="s">
         <v>56</v>
       </c>
@@ -43267,7 +43268,7 @@
       <c r="D167" s="20"/>
       <c r="E167" s="1"/>
     </row>
-    <row r="168" spans="2:8" ht="33.6">
+    <row r="168" spans="2:8" ht="33.75">
       <c r="B168" s="15" t="s">
         <v>74</v>
       </c>
@@ -43818,7 +43819,7 @@
       <c r="D202" s="20"/>
       <c r="E202" s="1"/>
     </row>
-    <row r="203" spans="2:7" ht="33.6">
+    <row r="203" spans="2:7" ht="33.75">
       <c r="B203" s="15" t="s">
         <v>99</v>
       </c>
@@ -44613,7 +44614,7 @@
         <v>1.0368820639798092E-2</v>
       </c>
     </row>
-    <row r="249" spans="2:5" ht="33.6">
+    <row r="249" spans="2:5" ht="33.75">
       <c r="B249" s="15" t="s">
         <v>111</v>
       </c>
@@ -45697,7 +45698,7 @@
         <v>1.3234596757570216E-2</v>
       </c>
     </row>
-    <row r="298" spans="2:11" ht="33.6">
+    <row r="298" spans="2:11" ht="33.75">
       <c r="B298" s="15" t="s">
         <v>128</v>
       </c>
@@ -46156,21 +46157,21 @@
       <selection activeCell="H344" sqref="H344"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="33.6">
+    <row r="2" spans="2:13" ht="33.75">
       <c r="B2" s="15" t="s">
         <v>144</v>
       </c>
@@ -49317,7 +49318,7 @@
         <v>-6.9805203823997616E-2</v>
       </c>
     </row>
-    <row r="110" spans="2:11" ht="33.6">
+    <row r="110" spans="2:11" ht="33.75">
       <c r="B110" s="15" t="s">
         <v>153</v>
       </c>
@@ -49338,7 +49339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="2:10" ht="28.8">
+    <row r="117" spans="2:10" ht="30">
       <c r="B117" t="s">
         <v>156</v>
       </c>
@@ -49496,8 +49497,8 @@
         <v>2.6453274055759479E-2</v>
       </c>
     </row>
-    <row r="125" spans="2:10" ht="15" thickBot="1"/>
-    <row r="126" spans="2:10" ht="28.8">
+    <row r="125" spans="2:10" ht="15.75" thickBot="1"/>
+    <row r="126" spans="2:10" ht="45">
       <c r="B126" t="s">
         <v>156</v>
       </c>
@@ -49665,7 +49666,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="132" spans="2:10" ht="15" thickBot="1">
+    <row r="132" spans="2:10" ht="15.75" thickBot="1">
       <c r="B132">
         <v>6</v>
       </c>
@@ -49693,7 +49694,7 @@
         <v>52963</v>
       </c>
     </row>
-    <row r="137" spans="2:10" ht="33.6">
+    <row r="137" spans="2:10" ht="33.75">
       <c r="B137" s="15" t="s">
         <v>177</v>
       </c>
@@ -49739,7 +49740,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="146" spans="2:10" ht="28.8">
+    <row r="146" spans="2:10" ht="30">
       <c r="B146" s="9" t="s">
         <v>174</v>
       </c>
@@ -50054,7 +50055,7 @@
         <v>21.00479034605814</v>
       </c>
     </row>
-    <row r="168" spans="2:10" ht="33.6">
+    <row r="168" spans="2:10" ht="33.75">
       <c r="B168" s="15" t="s">
         <v>180</v>
       </c>
@@ -50126,7 +50127,7 @@
         <v>21.903844753600076</v>
       </c>
     </row>
-    <row r="180" spans="2:4" ht="28.8">
+    <row r="180" spans="2:4" ht="30">
       <c r="B180" s="9" t="s">
         <v>184</v>
       </c>
@@ -50306,7 +50307,7 @@
         <v>23.67377406547174</v>
       </c>
     </row>
-    <row r="198" spans="2:4" ht="33.6">
+    <row r="198" spans="2:4" ht="33.75">
       <c r="B198" s="15" t="s">
         <v>187</v>
       </c>
@@ -50395,7 +50396,7 @@
         <v>825.37280366272546</v>
       </c>
     </row>
-    <row r="211" spans="2:6" ht="28.8">
+    <row r="211" spans="2:6" ht="30">
       <c r="B211" s="9" t="s">
         <v>184</v>
       </c>
@@ -50685,7 +50686,7 @@
         <v>49.317558304878645</v>
       </c>
     </row>
-    <row r="229" spans="2:4" ht="33.6">
+    <row r="229" spans="2:4" ht="33.75">
       <c r="B229" s="15" t="s">
         <v>193</v>
       </c>
@@ -50780,7 +50781,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="245" spans="2:6" ht="28.8">
+    <row r="245" spans="2:6" ht="30">
       <c r="B245" s="47" t="s">
         <v>195</v>
       </c>
@@ -51082,7 +51083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="2:4" ht="28.8">
+    <row r="278" spans="2:4" ht="30">
       <c r="B278" s="9" t="s">
         <v>199</v>
       </c>
@@ -51238,7 +51239,7 @@
         <v>926.21422626214394</v>
       </c>
     </row>
-    <row r="296" spans="2:12" ht="33.6">
+    <row r="296" spans="2:12" ht="33.75">
       <c r="B296" s="15" t="s">
         <v>201</v>
       </c>
@@ -51983,30 +51984,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:Q139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C99" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I108" sqref="I108:I124"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="33.6">
+    <row r="2" spans="2:15" ht="33.75">
       <c r="B2" s="15" t="s">
         <v>227</v>
       </c>
@@ -52153,7 +52154,7 @@
     <row r="14" spans="2:15">
       <c r="F14" s="17"/>
     </row>
-    <row r="17" spans="2:7" ht="33.6">
+    <row r="17" spans="2:7" ht="33.75">
       <c r="B17" s="15" t="s">
         <v>249</v>
       </c>
@@ -52428,7 +52429,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="33.6">
+    <row r="43" spans="2:7" ht="33.75">
       <c r="B43" s="15" t="s">
         <v>250</v>
       </c>
@@ -52836,7 +52837,7 @@
         <v>0.45326829053303058</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="33.6">
+    <row r="70" spans="2:7" ht="33.75">
       <c r="B70" s="15" t="s">
         <v>255</v>
       </c>
@@ -53208,7 +53209,7 @@
         <v>115.42063795932489</v>
       </c>
     </row>
-    <row r="103" spans="2:10" ht="33.6">
+    <row r="103" spans="2:10" ht="33.75">
       <c r="B103" s="15" t="s">
         <v>263</v>
       </c>
@@ -53232,6 +53233,9 @@
       <c r="H106" t="s">
         <v>266</v>
       </c>
+      <c r="I106" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="107" spans="2:10">
       <c r="B107">
@@ -53282,6 +53286,10 @@
         <f>H107*G108</f>
         <v>1.0287515225334958</v>
       </c>
+      <c r="I108">
+        <f>PRODUCT(G$108:G108)</f>
+        <v>1.0287515225334958</v>
+      </c>
       <c r="J108" s="24"/>
     </row>
     <row r="109" spans="2:10">
@@ -53310,6 +53318,10 @@
         <f t="shared" ref="H109:H125" si="7">H108*G109</f>
         <v>1.0610554192590551</v>
       </c>
+      <c r="I109">
+        <f>PRODUCT(G$108:G109)</f>
+        <v>1.0610554192590551</v>
+      </c>
       <c r="J109" s="24"/>
     </row>
     <row r="110" spans="2:10">
@@ -53338,6 +53350,10 @@
         <f t="shared" si="7"/>
         <v>1.0971281080058046</v>
       </c>
+      <c r="I110">
+        <f>PRODUCT(G$108:G110)</f>
+        <v>1.0971281080058046</v>
+      </c>
       <c r="J110" s="24"/>
     </row>
     <row r="111" spans="2:10">
@@ -53366,6 +53382,10 @@
         <f t="shared" si="7"/>
         <v>1.1373811872408448</v>
       </c>
+      <c r="I111">
+        <f>PRODUCT(G$108:G111)</f>
+        <v>1.1373811872408448</v>
+      </c>
       <c r="J111" s="24"/>
     </row>
     <row r="112" spans="2:10">
@@ -53394,6 +53414,10 @@
         <f t="shared" si="7"/>
         <v>1.1822547664097256</v>
       </c>
+      <c r="I112">
+        <f>PRODUCT(G$108:G112)</f>
+        <v>1.1822547664097256</v>
+      </c>
       <c r="J112" s="24"/>
     </row>
     <row r="113" spans="2:10">
@@ -53422,6 +53446,10 @@
         <f t="shared" si="7"/>
         <v>1.2322646508710511</v>
       </c>
+      <c r="I113">
+        <f>PRODUCT(G$108:G113)</f>
+        <v>1.2322646508710511</v>
+      </c>
       <c r="J113" s="24"/>
     </row>
     <row r="114" spans="2:10">
@@ -53450,6 +53478,10 @@
         <f t="shared" si="7"/>
         <v>1.2766640201593922</v>
       </c>
+      <c r="I114">
+        <f>PRODUCT(G$108:G114)</f>
+        <v>1.2766640201593922</v>
+      </c>
       <c r="J114" s="24"/>
     </row>
     <row r="115" spans="2:10">
@@ -53478,6 +53510,10 @@
         <f t="shared" si="7"/>
         <v>1.3335126793897147</v>
       </c>
+      <c r="I115">
+        <f>PRODUCT(G$108:G115)</f>
+        <v>1.3335126793897147</v>
+      </c>
       <c r="J115" s="24"/>
     </row>
     <row r="116" spans="2:10">
@@ -53506,6 +53542,10 @@
         <f t="shared" si="7"/>
         <v>1.3881603972601306</v>
       </c>
+      <c r="I116">
+        <f>PRODUCT(G$108:G116)</f>
+        <v>1.3881603972601306</v>
+      </c>
       <c r="J116" s="24"/>
     </row>
     <row r="117" spans="2:10">
@@ -53534,6 +53574,10 @@
         <f t="shared" si="7"/>
         <v>1.4420992072201613</v>
       </c>
+      <c r="I117">
+        <f>PRODUCT(G$108:G117)</f>
+        <v>1.4420992072201613</v>
+      </c>
       <c r="J117" s="24"/>
     </row>
     <row r="118" spans="2:10">
@@ -53562,6 +53606,10 @@
         <f t="shared" si="7"/>
         <v>1.4990460627417292</v>
       </c>
+      <c r="I118">
+        <f>PRODUCT(G$108:G118)</f>
+        <v>1.4990460627417292</v>
+      </c>
       <c r="J118" s="24"/>
     </row>
     <row r="119" spans="2:10">
@@ -53590,6 +53638,10 @@
         <f t="shared" si="7"/>
         <v>1.5654673746835543</v>
       </c>
+      <c r="I119">
+        <f>PRODUCT(G$108:G119)</f>
+        <v>1.5654673746835543</v>
+      </c>
       <c r="J119" s="24"/>
     </row>
     <row r="120" spans="2:10">
@@ -53618,6 +53670,10 @@
         <f t="shared" si="7"/>
         <v>1.6297692203890721</v>
       </c>
+      <c r="I120">
+        <f>PRODUCT(G$108:G120)</f>
+        <v>1.6297692203890721</v>
+      </c>
       <c r="J120" s="24"/>
     </row>
     <row r="121" spans="2:10">
@@ -53646,6 +53702,10 @@
         <f t="shared" si="7"/>
         <v>1.6978385894893901</v>
       </c>
+      <c r="I121">
+        <f>PRODUCT(G$108:G121)</f>
+        <v>1.6978385894893901</v>
+      </c>
       <c r="J121" s="24"/>
     </row>
     <row r="122" spans="2:10">
@@ -53674,6 +53734,10 @@
         <f t="shared" si="7"/>
         <v>1.7793590003090549</v>
       </c>
+      <c r="I122">
+        <f>PRODUCT(G$108:G122)</f>
+        <v>1.7793590003090549</v>
+      </c>
       <c r="J122" s="24"/>
     </row>
     <row r="123" spans="2:10">
@@ -53702,6 +53766,10 @@
         <f t="shared" si="7"/>
         <v>1.8675442018038635</v>
       </c>
+      <c r="I123">
+        <f>PRODUCT(G$108:G123)</f>
+        <v>1.8675442018038635</v>
+      </c>
       <c r="J123" s="24"/>
     </row>
     <row r="124" spans="2:10">
@@ -53730,6 +53798,10 @@
         <f t="shared" si="7"/>
         <v>1.9385108814724088</v>
       </c>
+      <c r="I124">
+        <f>PRODUCT(G$108:G124)</f>
+        <v>1.9385108814724088</v>
+      </c>
       <c r="J124" s="24"/>
     </row>
     <row r="125" spans="2:10">
@@ -53758,6 +53830,10 @@
         <f t="shared" si="7"/>
         <v>2.0396970999828001</v>
       </c>
+      <c r="I125">
+        <f>PRODUCT(G$108:G125)</f>
+        <v>2.0396970999828001</v>
+      </c>
       <c r="J125" s="24"/>
     </row>
     <row r="126" spans="2:10">
@@ -53772,7 +53848,7 @@
       </c>
       <c r="E126" s="33"/>
     </row>
-    <row r="130" spans="1:17" ht="33.6">
+    <row r="130" spans="1:17" ht="33.75">
       <c r="B130" s="15" t="s">
         <v>289</v>
       </c>

</xml_diff>

<commit_message>
[BAF510] :  채권 엑셀 정리
</commit_message>
<xml_diff>
--- a/BAF510채권/T2.xlsx
+++ b/BAF510채권/T2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chlje\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6A6A90-90BB-4E9D-AB7D-79C789D13B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70273B10-164C-44AA-8769-62172EED503D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price" sheetId="1" r:id="rId1"/>
@@ -36201,14 +36201,14 @@
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="33.75">
+    <row r="2" spans="2:4" ht="33.6">
       <c r="B2" s="15" t="s">
         <v>292</v>
       </c>
@@ -36301,7 +36301,7 @@
         <v>1156.8950957737293</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="15.75" thickBot="1"/>
+    <row r="25" spans="2:16" ht="15" thickBot="1"/>
     <row r="26" spans="2:16">
       <c r="B26" s="2" t="s">
         <v>3</v>
@@ -36379,7 +36379,7 @@
         <v>1150.8261172101793</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="15.75" thickBot="1">
+    <row r="30" spans="2:16" ht="15" thickBot="1">
       <c r="B30" s="6" t="s">
         <v>7</v>
       </c>
@@ -36414,7 +36414,7 @@
         <v>1854.4338616001187</v>
       </c>
     </row>
-    <row r="31" spans="2:16" ht="15.75" thickBot="1">
+    <row r="31" spans="2:16" ht="15" thickBot="1">
       <c r="E31">
         <v>19.5</v>
       </c>
@@ -36604,7 +36604,7 @@
         <v>1490.5430003379133</v>
       </c>
     </row>
-    <row r="37" spans="2:16" ht="15.75" thickBot="1">
+    <row r="37" spans="2:16" ht="15" thickBot="1">
       <c r="B37" s="6" t="s">
         <v>10</v>
       </c>
@@ -37206,17 +37206,17 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1"/>
+    <row r="1" spans="2:12" ht="15" thickBot="1"/>
     <row r="2" spans="2:12">
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -37250,7 +37250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="45">
+    <row r="5" spans="2:12" ht="43.2">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -37282,7 +37282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="15.75" thickBot="1">
+    <row r="6" spans="2:12" ht="15" thickBot="1">
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
@@ -37321,7 +37321,7 @@
         <v>940.37050780850541</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1">
+    <row r="7" spans="2:12" ht="15" thickBot="1">
       <c r="E7">
         <f>E6-0.1</f>
         <v>9.8000000000000007</v>
@@ -37560,7 +37560,7 @@
         <v>942.3526434574311</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="15.75" thickBot="1">
+    <row r="13" spans="2:12" ht="15" thickBot="1">
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
@@ -40710,21 +40710,21 @@
       <selection activeCell="G267" sqref="G267"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="33.75">
+    <row r="2" spans="2:10" ht="33.6">
       <c r="B2" s="15" t="s">
         <v>29</v>
       </c>
@@ -40974,12 +40974,12 @@
         <v>-210.19876543209875</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="33.75">
+    <row r="30" spans="2:10" ht="33.6">
       <c r="B30" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="45">
+    <row r="33" spans="2:8" ht="43.2">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -41198,7 +41198,7 @@
         <v>6492830.2486569844</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="33.75">
+    <row r="51" spans="2:12" ht="33.6">
       <c r="B51" s="15" t="s">
         <v>40</v>
       </c>
@@ -42067,7 +42067,7 @@
     <row r="86" spans="2:12">
       <c r="D86" s="19"/>
     </row>
-    <row r="89" spans="2:12" ht="33.75">
+    <row r="89" spans="2:12" ht="33.6">
       <c r="B89" s="15" t="s">
         <v>50</v>
       </c>
@@ -42351,7 +42351,7 @@
         <v>-5.8692194215836935E-7</v>
       </c>
     </row>
-    <row r="113" spans="2:11" ht="33.75">
+    <row r="113" spans="2:11" ht="33.6">
       <c r="B113" s="15" t="s">
         <v>56</v>
       </c>
@@ -43268,7 +43268,7 @@
       <c r="D167" s="20"/>
       <c r="E167" s="1"/>
     </row>
-    <row r="168" spans="2:8" ht="33.75">
+    <row r="168" spans="2:8" ht="33.6">
       <c r="B168" s="15" t="s">
         <v>74</v>
       </c>
@@ -43819,7 +43819,7 @@
       <c r="D202" s="20"/>
       <c r="E202" s="1"/>
     </row>
-    <row r="203" spans="2:7" ht="33.75">
+    <row r="203" spans="2:7" ht="33.6">
       <c r="B203" s="15" t="s">
         <v>99</v>
       </c>
@@ -44614,7 +44614,7 @@
         <v>1.0368820639798092E-2</v>
       </c>
     </row>
-    <row r="249" spans="2:5" ht="33.75">
+    <row r="249" spans="2:5" ht="33.6">
       <c r="B249" s="15" t="s">
         <v>111</v>
       </c>
@@ -45698,7 +45698,7 @@
         <v>1.3234596757570216E-2</v>
       </c>
     </row>
-    <row r="298" spans="2:11" ht="33.75">
+    <row r="298" spans="2:11" ht="33.6">
       <c r="B298" s="15" t="s">
         <v>128</v>
       </c>
@@ -46157,21 +46157,21 @@
       <selection activeCell="H344" sqref="H344"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="33.75">
+    <row r="2" spans="2:13" ht="33.6">
       <c r="B2" s="15" t="s">
         <v>144</v>
       </c>
@@ -49318,7 +49318,7 @@
         <v>-6.9805203823997616E-2</v>
       </c>
     </row>
-    <row r="110" spans="2:11" ht="33.75">
+    <row r="110" spans="2:11" ht="33.6">
       <c r="B110" s="15" t="s">
         <v>153</v>
       </c>
@@ -49339,7 +49339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="2:10" ht="30">
+    <row r="117" spans="2:10" ht="28.8">
       <c r="B117" t="s">
         <v>156</v>
       </c>
@@ -49497,8 +49497,8 @@
         <v>2.6453274055759479E-2</v>
       </c>
     </row>
-    <row r="125" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="126" spans="2:10" ht="45">
+    <row r="125" spans="2:10" ht="15" thickBot="1"/>
+    <row r="126" spans="2:10" ht="28.8">
       <c r="B126" t="s">
         <v>156</v>
       </c>
@@ -49666,7 +49666,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="132" spans="2:10" ht="15.75" thickBot="1">
+    <row r="132" spans="2:10" ht="15" thickBot="1">
       <c r="B132">
         <v>6</v>
       </c>
@@ -49694,7 +49694,7 @@
         <v>52963</v>
       </c>
     </row>
-    <row r="137" spans="2:10" ht="33.75">
+    <row r="137" spans="2:10" ht="33.6">
       <c r="B137" s="15" t="s">
         <v>177</v>
       </c>
@@ -49740,7 +49740,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="146" spans="2:10" ht="30">
+    <row r="146" spans="2:10" ht="28.8">
       <c r="B146" s="9" t="s">
         <v>174</v>
       </c>
@@ -50055,7 +50055,7 @@
         <v>21.00479034605814</v>
       </c>
     </row>
-    <row r="168" spans="2:10" ht="33.75">
+    <row r="168" spans="2:10" ht="33.6">
       <c r="B168" s="15" t="s">
         <v>180</v>
       </c>
@@ -50127,7 +50127,7 @@
         <v>21.903844753600076</v>
       </c>
     </row>
-    <row r="180" spans="2:4" ht="30">
+    <row r="180" spans="2:4" ht="28.8">
       <c r="B180" s="9" t="s">
         <v>184</v>
       </c>
@@ -50307,7 +50307,7 @@
         <v>23.67377406547174</v>
       </c>
     </row>
-    <row r="198" spans="2:4" ht="33.75">
+    <row r="198" spans="2:4" ht="33.6">
       <c r="B198" s="15" t="s">
         <v>187</v>
       </c>
@@ -50396,7 +50396,7 @@
         <v>825.37280366272546</v>
       </c>
     </row>
-    <row r="211" spans="2:6" ht="30">
+    <row r="211" spans="2:6" ht="28.8">
       <c r="B211" s="9" t="s">
         <v>184</v>
       </c>
@@ -50686,7 +50686,7 @@
         <v>49.317558304878645</v>
       </c>
     </row>
-    <row r="229" spans="2:4" ht="33.75">
+    <row r="229" spans="2:4" ht="33.6">
       <c r="B229" s="15" t="s">
         <v>193</v>
       </c>
@@ -50781,7 +50781,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="245" spans="2:6" ht="30">
+    <row r="245" spans="2:6" ht="28.8">
       <c r="B245" s="47" t="s">
         <v>195</v>
       </c>
@@ -51083,7 +51083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="2:4" ht="30">
+    <row r="278" spans="2:4" ht="28.8">
       <c r="B278" s="9" t="s">
         <v>199</v>
       </c>
@@ -51239,7 +51239,7 @@
         <v>926.21422626214394</v>
       </c>
     </row>
-    <row r="296" spans="2:12" ht="33.75">
+    <row r="296" spans="2:12" ht="33.6">
       <c r="B296" s="15" t="s">
         <v>201</v>
       </c>
@@ -51984,30 +51984,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:Q139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I110" sqref="I110"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="33.75">
+    <row r="2" spans="2:15" ht="33.6">
       <c r="B2" s="15" t="s">
         <v>227</v>
       </c>
@@ -52154,7 +52154,7 @@
     <row r="14" spans="2:15">
       <c r="F14" s="17"/>
     </row>
-    <row r="17" spans="2:7" ht="33.75">
+    <row r="17" spans="2:7" ht="33.6">
       <c r="B17" s="15" t="s">
         <v>249</v>
       </c>
@@ -52429,7 +52429,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="33.75">
+    <row r="43" spans="2:7" ht="33.6">
       <c r="B43" s="15" t="s">
         <v>250</v>
       </c>
@@ -52837,7 +52837,7 @@
         <v>0.45326829053303058</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="33.75">
+    <row r="70" spans="2:7" ht="33.6">
       <c r="B70" s="15" t="s">
         <v>255</v>
       </c>
@@ -53209,7 +53209,7 @@
         <v>115.42063795932489</v>
       </c>
     </row>
-    <row r="103" spans="2:10" ht="33.75">
+    <row r="103" spans="2:10" ht="33.6">
       <c r="B103" s="15" t="s">
         <v>263</v>
       </c>
@@ -53848,7 +53848,7 @@
       </c>
       <c r="E126" s="33"/>
     </row>
-    <row r="130" spans="1:17" ht="33.75">
+    <row r="130" spans="1:17" ht="33.6">
       <c r="B130" s="15" t="s">
         <v>289</v>
       </c>

</xml_diff>

<commit_message>
[BAF510] : volatility > price-yield relationship 컬러 스케일 시각화
</commit_message>
<xml_diff>
--- a/BAF510채권/T2.xlsx
+++ b/BAF510채권/T2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chlje\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70273B10-164C-44AA-8769-62172EED503D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DBE6DD-0417-4C58-B4CC-D8B28C34FE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price" sheetId="1" r:id="rId1"/>
@@ -36201,14 +36201,14 @@
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="33.6">
+    <row r="2" spans="2:4" ht="33.75">
       <c r="B2" s="15" t="s">
         <v>292</v>
       </c>
@@ -36301,7 +36301,7 @@
         <v>1156.8950957737293</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="15" thickBot="1"/>
+    <row r="25" spans="2:16" ht="15.75" thickBot="1"/>
     <row r="26" spans="2:16">
       <c r="B26" s="2" t="s">
         <v>3</v>
@@ -36379,7 +36379,7 @@
         <v>1150.8261172101793</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="15" thickBot="1">
+    <row r="30" spans="2:16" ht="15.75" thickBot="1">
       <c r="B30" s="6" t="s">
         <v>7</v>
       </c>
@@ -36403,18 +36403,18 @@
         <v>20</v>
       </c>
       <c r="L30" s="1">
-        <f t="dataTable" ref="L30:L70" dt2D="0" dtr="0" r1="I27" ca="1"/>
+        <f t="dataTable" ref="L30:L70" dt2D="0" dtr="0" r1="I27"/>
         <v>1220.9983991771542</v>
       </c>
       <c r="O30">
         <v>0.01</v>
       </c>
       <c r="P30">
-        <f t="dataTable" ref="P30:P52" dt2D="0" dtr="0" r1="I30"/>
+        <f t="dataTable" ref="P30:P52" dt2D="0" dtr="0" r1="I30" ca="1"/>
         <v>1854.4338616001187</v>
       </c>
     </row>
-    <row r="31" spans="2:16" ht="15" thickBot="1">
+    <row r="31" spans="2:16" ht="15.75" thickBot="1">
       <c r="E31">
         <v>19.5</v>
       </c>
@@ -36604,7 +36604,7 @@
         <v>1490.5430003379133</v>
       </c>
     </row>
-    <row r="37" spans="2:16" ht="15" thickBot="1">
+    <row r="37" spans="2:16" ht="15.75" thickBot="1">
       <c r="B37" s="6" t="s">
         <v>10</v>
       </c>
@@ -37206,17 +37206,17 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1"/>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:12">
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -37250,7 +37250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="43.2">
+    <row r="5" spans="2:12" ht="45">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -37282,7 +37282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="15" thickBot="1">
+    <row r="6" spans="2:12" ht="15.75" thickBot="1">
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
@@ -37321,7 +37321,7 @@
         <v>940.37050780850541</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15" thickBot="1">
+    <row r="7" spans="2:12" ht="15.75" thickBot="1">
       <c r="E7">
         <f>E6-0.1</f>
         <v>9.8000000000000007</v>
@@ -37560,7 +37560,7 @@
         <v>942.3526434574311</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="15" thickBot="1">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1">
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
@@ -40706,25 +40706,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:N329"/>
   <sheetViews>
-    <sheetView topLeftCell="A249" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A309" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G267" sqref="G267"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="33.6">
+    <row r="2" spans="2:10" ht="33.75">
       <c r="B2" s="15" t="s">
         <v>29</v>
       </c>
@@ -40974,12 +40974,12 @@
         <v>-210.19876543209875</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="33.6">
+    <row r="30" spans="2:10" ht="33.75">
       <c r="B30" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="43.2">
+    <row r="33" spans="2:8" ht="45">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -41198,7 +41198,7 @@
         <v>6492830.2486569844</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="33.6">
+    <row r="51" spans="2:12" ht="33.75">
       <c r="B51" s="15" t="s">
         <v>40</v>
       </c>
@@ -42067,7 +42067,7 @@
     <row r="86" spans="2:12">
       <c r="D86" s="19"/>
     </row>
-    <row r="89" spans="2:12" ht="33.6">
+    <row r="89" spans="2:12" ht="33.75">
       <c r="B89" s="15" t="s">
         <v>50</v>
       </c>
@@ -42351,7 +42351,7 @@
         <v>-5.8692194215836935E-7</v>
       </c>
     </row>
-    <row r="113" spans="2:11" ht="33.6">
+    <row r="113" spans="2:11" ht="33.75">
       <c r="B113" s="15" t="s">
         <v>56</v>
       </c>
@@ -43268,7 +43268,7 @@
       <c r="D167" s="20"/>
       <c r="E167" s="1"/>
     </row>
-    <row r="168" spans="2:8" ht="33.6">
+    <row r="168" spans="2:8" ht="33.75">
       <c r="B168" s="15" t="s">
         <v>74</v>
       </c>
@@ -43819,7 +43819,7 @@
       <c r="D202" s="20"/>
       <c r="E202" s="1"/>
     </row>
-    <row r="203" spans="2:7" ht="33.6">
+    <row r="203" spans="2:7" ht="33.75">
       <c r="B203" s="15" t="s">
         <v>99</v>
       </c>
@@ -44614,7 +44614,7 @@
         <v>1.0368820639798092E-2</v>
       </c>
     </row>
-    <row r="249" spans="2:5" ht="33.6">
+    <row r="249" spans="2:5" ht="33.75">
       <c r="B249" s="15" t="s">
         <v>111</v>
       </c>
@@ -45698,7 +45698,7 @@
         <v>1.3234596757570216E-2</v>
       </c>
     </row>
-    <row r="298" spans="2:11" ht="33.6">
+    <row r="298" spans="2:11" ht="33.75">
       <c r="B298" s="15" t="s">
         <v>128</v>
       </c>
@@ -46153,25 +46153,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:M354"/>
   <sheetViews>
-    <sheetView topLeftCell="A288" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H344" sqref="H344"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L97" sqref="L97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="33.6">
+    <row r="2" spans="2:13" ht="33.75">
       <c r="B2" s="15" t="s">
         <v>144</v>
       </c>
@@ -49318,7 +49318,7 @@
         <v>-6.9805203823997616E-2</v>
       </c>
     </row>
-    <row r="110" spans="2:11" ht="33.6">
+    <row r="110" spans="2:11" ht="33.75">
       <c r="B110" s="15" t="s">
         <v>153</v>
       </c>
@@ -49339,7 +49339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="2:10" ht="28.8">
+    <row r="117" spans="2:10" ht="30">
       <c r="B117" t="s">
         <v>156</v>
       </c>
@@ -49497,8 +49497,8 @@
         <v>2.6453274055759479E-2</v>
       </c>
     </row>
-    <row r="125" spans="2:10" ht="15" thickBot="1"/>
-    <row r="126" spans="2:10" ht="28.8">
+    <row r="125" spans="2:10" ht="15.75" thickBot="1"/>
+    <row r="126" spans="2:10" ht="45">
       <c r="B126" t="s">
         <v>156</v>
       </c>
@@ -49666,7 +49666,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="132" spans="2:10" ht="15" thickBot="1">
+    <row r="132" spans="2:10" ht="15.75" thickBot="1">
       <c r="B132">
         <v>6</v>
       </c>
@@ -49694,7 +49694,7 @@
         <v>52963</v>
       </c>
     </row>
-    <row r="137" spans="2:10" ht="33.6">
+    <row r="137" spans="2:10" ht="33.75">
       <c r="B137" s="15" t="s">
         <v>177</v>
       </c>
@@ -49740,7 +49740,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="146" spans="2:10" ht="28.8">
+    <row r="146" spans="2:10" ht="30">
       <c r="B146" s="9" t="s">
         <v>174</v>
       </c>
@@ -50055,7 +50055,7 @@
         <v>21.00479034605814</v>
       </c>
     </row>
-    <row r="168" spans="2:10" ht="33.6">
+    <row r="168" spans="2:10" ht="33.75">
       <c r="B168" s="15" t="s">
         <v>180</v>
       </c>
@@ -50127,7 +50127,7 @@
         <v>21.903844753600076</v>
       </c>
     </row>
-    <row r="180" spans="2:4" ht="28.8">
+    <row r="180" spans="2:4" ht="30">
       <c r="B180" s="9" t="s">
         <v>184</v>
       </c>
@@ -50307,7 +50307,7 @@
         <v>23.67377406547174</v>
       </c>
     </row>
-    <row r="198" spans="2:4" ht="33.6">
+    <row r="198" spans="2:4" ht="33.75">
       <c r="B198" s="15" t="s">
         <v>187</v>
       </c>
@@ -50396,7 +50396,7 @@
         <v>825.37280366272546</v>
       </c>
     </row>
-    <row r="211" spans="2:6" ht="28.8">
+    <row r="211" spans="2:6" ht="30">
       <c r="B211" s="9" t="s">
         <v>184</v>
       </c>
@@ -50686,7 +50686,7 @@
         <v>49.317558304878645</v>
       </c>
     </row>
-    <row r="229" spans="2:4" ht="33.6">
+    <row r="229" spans="2:4" ht="33.75">
       <c r="B229" s="15" t="s">
         <v>193</v>
       </c>
@@ -50781,7 +50781,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="245" spans="2:6" ht="28.8">
+    <row r="245" spans="2:6" ht="30">
       <c r="B245" s="47" t="s">
         <v>195</v>
       </c>
@@ -50802,14 +50802,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="C246">
-        <f t="dataTable" ref="C246:C258" dt2D="0" dtr="0" r1="C237" ca="1"/>
+        <f t="dataTable" ref="C246:C258" dt2D="0" dtr="0" r1="C237"/>
         <v>1631.5889067095873</v>
       </c>
       <c r="E246">
         <v>0</v>
       </c>
       <c r="F246">
-        <f t="dataTable" ref="F246:F258" dt2D="0" dtr="0" r1="C235"/>
+        <f t="dataTable" ref="F246:F258" dt2D="0" dtr="0" r1="C235" ca="1"/>
         <v>3351.5716215288121</v>
       </c>
     </row>
@@ -51083,7 +51083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="2:4" ht="28.8">
+    <row r="278" spans="2:4" ht="30">
       <c r="B278" s="9" t="s">
         <v>199</v>
       </c>
@@ -51239,7 +51239,7 @@
         <v>926.21422626214394</v>
       </c>
     </row>
-    <row r="296" spans="2:12" ht="33.6">
+    <row r="296" spans="2:12" ht="33.75">
       <c r="B296" s="15" t="s">
         <v>201</v>
       </c>
@@ -51975,6 +51975,64 @@
     <mergeCell ref="I127:I132"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C10:M22">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="100"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color theme="0"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:M40">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color theme="0"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:K63">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="100"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color theme="0"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C69:K81">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color theme="0"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C92:K103">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -51984,30 +52042,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:Q139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="33.6">
+    <row r="2" spans="2:15" ht="33.75">
       <c r="B2" s="15" t="s">
         <v>227</v>
       </c>
@@ -52154,7 +52212,7 @@
     <row r="14" spans="2:15">
       <c r="F14" s="17"/>
     </row>
-    <row r="17" spans="2:7" ht="33.6">
+    <row r="17" spans="2:7" ht="33.75">
       <c r="B17" s="15" t="s">
         <v>249</v>
       </c>
@@ -52429,7 +52487,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="33.6">
+    <row r="43" spans="2:7" ht="33.75">
       <c r="B43" s="15" t="s">
         <v>250</v>
       </c>
@@ -52837,7 +52895,7 @@
         <v>0.45326829053303058</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="33.6">
+    <row r="70" spans="2:7" ht="33.75">
       <c r="B70" s="15" t="s">
         <v>255</v>
       </c>
@@ -53209,7 +53267,7 @@
         <v>115.42063795932489</v>
       </c>
     </row>
-    <row r="103" spans="2:10" ht="33.6">
+    <row r="103" spans="2:10" ht="33.75">
       <c r="B103" s="15" t="s">
         <v>263</v>
       </c>
@@ -53848,7 +53906,7 @@
       </c>
       <c r="E126" s="33"/>
     </row>
-    <row r="130" spans="1:17" ht="33.6">
+    <row r="130" spans="1:17" ht="33.75">
       <c r="B130" s="15" t="s">
         <v>289</v>
       </c>

</xml_diff>